<commit_message>
excel planification document update
</commit_message>
<xml_diff>
--- a/docs/C61 - Sprint1c - Outil de planification.xlsx
+++ b/docs/C61 - Sprint1c - Outil de planification.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1649508\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1649508\Downloads\GreenFlag\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DDDFAB9-1AF7-4332-841E-43F31634E966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6949BBF6-31EE-4896-BEC4-495DA666B2A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -383,7 +383,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="113">
   <si>
     <t>Planification</t>
   </si>
@@ -748,9 +748,6 @@
     <t>Création des squelettes des classes en backend</t>
   </si>
   <si>
-    <t>Composantes React: Home, Login, Create account page, Questionnaire page</t>
-  </si>
-  <si>
     <t>Authentification backend avec la création des token &amp; decorateur token_required</t>
   </si>
   <si>
@@ -760,13 +757,97 @@
     <t>les DAO</t>
   </si>
   <si>
-    <t>les Manager: Account, Matching, Notification</t>
-  </si>
-  <si>
     <t>ChatroomManager et websocket</t>
   </si>
   <si>
-    <t>Page de suggestions en React (sans swipe, juste boutons)</t>
+    <t>backend: abstract Strategy + AlgoStrategy</t>
+  </si>
+  <si>
+    <t>bibliotheque: Queue</t>
+  </si>
+  <si>
+    <t>bibliotheque: middleware</t>
+  </si>
+  <si>
+    <t>trigger &amp; fonction pour tableau suggestion dans la base de données</t>
+  </si>
+  <si>
+    <t>page Statistiques React</t>
+  </si>
+  <si>
+    <t>classe Statistics backend + fonctions statistiques base de données</t>
+  </si>
+  <si>
+    <t>Composantes React: Home, Login, Create account page, Questionnaire page - de base</t>
+  </si>
+  <si>
+    <t>Page de suggestions en React (sans swipe, juste boutons) - de base</t>
+  </si>
+  <si>
+    <t>Chatrooms Page React de base</t>
+  </si>
+  <si>
+    <t>Private chatroom page React de base</t>
+  </si>
+  <si>
+    <t>TestSimulator + UserFactory 1ere version</t>
+  </si>
+  <si>
+    <t>les Manager: Account, Matching</t>
+  </si>
+  <si>
+    <t>NotificationManager</t>
+  </si>
+  <si>
+    <t>classe User</t>
+  </si>
+  <si>
+    <t>EmailAdapter</t>
+  </si>
+  <si>
+    <t>Implementation des autres algorithmes en librairie et plugger dans Strategy</t>
+  </si>
+  <si>
+    <t>Ameliorer page de Suggestions - React</t>
+  </si>
+  <si>
+    <t>Amelioration des pages de Login, Create Account - React</t>
+  </si>
+  <si>
+    <t>Ameliorer tous les composantes de Bouton et les Icones - React</t>
+  </si>
+  <si>
+    <t>Ameliorer page de private chatroom</t>
+  </si>
+  <si>
+    <t>TestSimulator + UserFactory 2eme version</t>
+  </si>
+  <si>
+    <t>Reviser la logique interne de l'entiereté du programme</t>
+  </si>
+  <si>
+    <t>SwipingStrategy</t>
+  </si>
+  <si>
+    <t>Fonctionnalité de flagging</t>
+  </si>
+  <si>
+    <t>Page de modification de profil</t>
+  </si>
+  <si>
+    <t>Rapport final</t>
+  </si>
+  <si>
+    <t>Readme</t>
+  </si>
+  <si>
+    <t>Vidéo de présentation</t>
+  </si>
+  <si>
+    <t>API localisation dans le frontend + introduction dans l'algo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pages de confirmation email, page de menu (settings) </t>
   </si>
 </sst>
 </file>
@@ -1030,7 +1111,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1143,18 +1224,18 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1171,11 +1252,15 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1646,13 +1731,13 @@
                   <c:v>1.8645833333294597</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.95833333333333437</c:v>
+                  <c:v>1.7499999999999978</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1.7187500000000153</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.96875000000000144</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2049,10 +2134,10 @@
                 <c:formatCode>[hh]:mm</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>11</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.95833333333333437</c:v>
+                  <c:v>1.7499999999999978</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2166,10 +2251,10 @@
                 <c:formatCode>[hh]:mm</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1.7187500000000153</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2285,10 +2370,10 @@
                 <c:formatCode>[hh]:mm</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.96875000000000144</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2621,10 +2706,10 @@
                 <c:formatCode>[hh]:mm</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>15</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.8229166666627945</c:v>
+                  <c:v>5.9479166666628061</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2680,10 +2765,10 @@
                 <c:formatCode>[hh]:mm</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.22916666666666702</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2739,10 +2824,10 @@
                 <c:formatCode>[hh]:mm</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.125</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3074,10 +3159,10 @@
                 <c:formatCode>[hh]:mm</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>5</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.20833333333333345</c:v>
+                  <c:v>1.3854166666666685</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3133,10 +3218,10 @@
                 <c:formatCode>[hh]:mm</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>4</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.62500000000002309</c:v>
+                  <c:v>2.1666666666666896</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3192,10 +3277,10 @@
                 <c:formatCode>[hh]:mm</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9895833333294375</c:v>
+                  <c:v>2.749999999996116</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3527,10 +3612,10 @@
                 <c:formatCode>[hh]:mm</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>5</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.54166666666668972</c:v>
+                  <c:v>2.3437500000000249</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3586,10 +3671,10 @@
                 <c:formatCode>[hh]:mm</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.8333333333294373</c:v>
+                  <c:v>2.6666666666627665</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3645,10 +3730,10 @@
                 <c:formatCode>[hh]:mm</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>4</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.44791666666666741</c:v>
+                  <c:v>1.2916666666666825</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7420,8 +7505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AF97"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A23" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54:G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.26953125" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
@@ -7595,7 +7680,7 @@
       <c r="N13" s="46"/>
       <c r="U13" s="2">
         <f>D68</f>
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="AA13" s="2">
         <f>N7</f>
@@ -7607,12 +7692,12 @@
       <c r="C15" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="40" t="s">
+      <c r="D15" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="48"/>
       <c r="H15" s="5" t="s">
         <v>11</v>
       </c>
@@ -7663,12 +7748,12 @@
       <c r="C16" s="11">
         <v>1</v>
       </c>
-      <c r="D16" s="41" t="s">
+      <c r="D16" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="41"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="49"/>
       <c r="H16" s="30"/>
       <c r="I16" s="30" t="s">
         <v>17</v>
@@ -7707,12 +7792,12 @@
       <c r="C17" s="12">
         <v>2</v>
       </c>
-      <c r="D17" s="42" t="s">
+      <c r="D17" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
       <c r="H17" s="32">
         <v>1</v>
       </c>
@@ -7776,12 +7861,12 @@
       <c r="C18" s="13">
         <v>3</v>
       </c>
-      <c r="D18" s="39" t="s">
+      <c r="D18" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="39"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42"/>
       <c r="H18" s="34">
         <v>2</v>
       </c>
@@ -7838,23 +7923,23 @@
       </c>
       <c r="AD18" s="1">
         <f>COUNTIF(Sprint,AC18)</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="AE18" s="19">
         <f>SUMIFS(Duree, Sprint,AC18)</f>
-        <v>0.95833333333333437</v>
+        <v>1.7499999999999978</v>
       </c>
     </row>
     <row r="19" spans="3:31" x14ac:dyDescent="0.3">
       <c r="C19" s="12">
         <v>4</v>
       </c>
-      <c r="D19" s="42" t="s">
+      <c r="D19" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="E19" s="42"/>
-      <c r="F19" s="42"/>
-      <c r="G19" s="42"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
       <c r="H19" s="32">
         <v>3</v>
       </c>
@@ -7911,23 +7996,23 @@
       </c>
       <c r="AD19" s="1">
         <f>COUNTIF(Sprint,AC19)</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="AE19" s="19">
         <f>SUMIFS(Duree, Sprint,AC19)</f>
-        <v>0</v>
+        <v>1.7187500000000153</v>
       </c>
     </row>
     <row r="20" spans="3:31" x14ac:dyDescent="0.3">
       <c r="C20" s="13">
         <v>5</v>
       </c>
-      <c r="D20" s="39" t="s">
+      <c r="D20" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="E20" s="39"/>
-      <c r="F20" s="39"/>
-      <c r="G20" s="39"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="42"/>
+      <c r="G20" s="42"/>
       <c r="H20" s="34"/>
       <c r="I20" s="34" t="s">
         <v>17</v>
@@ -7970,23 +8055,23 @@
       </c>
       <c r="AD20" s="1">
         <f>COUNTIF(Sprint,AC20)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AE20" s="19">
         <f>SUMIFS(Duree, Sprint,AC20)</f>
-        <v>0</v>
+        <v>0.96875000000000144</v>
       </c>
     </row>
     <row r="21" spans="3:31" x14ac:dyDescent="0.3">
       <c r="C21" s="12">
         <v>6</v>
       </c>
-      <c r="D21" s="42" t="s">
+      <c r="D21" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="E21" s="42"/>
-      <c r="F21" s="42"/>
-      <c r="G21" s="42"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="41"/>
+      <c r="G21" s="41"/>
       <c r="H21" s="32">
         <v>5</v>
       </c>
@@ -8027,12 +8112,12 @@
       <c r="C22" s="13">
         <v>7</v>
       </c>
-      <c r="D22" s="39" t="s">
+      <c r="D22" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="E22" s="39"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="39"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="42"/>
       <c r="H22" s="34">
         <v>5</v>
       </c>
@@ -8069,12 +8154,12 @@
       <c r="C23" s="12">
         <v>8</v>
       </c>
-      <c r="D23" s="49" t="s">
+      <c r="D23" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="E23" s="49"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="49"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="40"/>
       <c r="H23" s="32">
         <v>5</v>
       </c>
@@ -8120,12 +8205,12 @@
       <c r="C24" s="13">
         <v>9</v>
       </c>
-      <c r="D24" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="E24" s="39"/>
-      <c r="F24" s="39"/>
-      <c r="G24" s="39"/>
+      <c r="D24" s="42" t="s">
+        <v>96</v>
+      </c>
+      <c r="E24" s="42"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="42"/>
       <c r="H24" s="34">
         <v>6</v>
       </c>
@@ -8133,19 +8218,19 @@
         <v>17</v>
       </c>
       <c r="J24" s="34">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K24" s="34">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L24" s="35">
-        <v>0.14583333333333401</v>
+        <v>3.125E-2</v>
       </c>
       <c r="M24" s="34" t="s">
         <v>14</v>
       </c>
       <c r="N24" s="34" t="s">
-        <v>73</v>
+        <v>21</v>
       </c>
       <c r="T24" s="1" t="b">
         <f t="shared" si="1"/>
@@ -8163,25 +8248,25 @@
       </c>
       <c r="AD24" s="1">
         <f>COUNTIF(Responsabilite,AC24)</f>
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="AE24" s="19">
         <f>SUMIFS(Duree, Responsabilite,AC24)</f>
-        <v>2.0312499999961267</v>
+        <v>3.7395833333294766</v>
       </c>
     </row>
     <row r="25" spans="3:31" x14ac:dyDescent="0.3">
       <c r="C25" s="12">
         <v>10</v>
       </c>
-      <c r="D25" s="42" t="s">
-        <v>80</v>
-      </c>
-      <c r="E25" s="42"/>
-      <c r="F25" s="42"/>
-      <c r="G25" s="42"/>
+      <c r="D25" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="E25" s="41"/>
+      <c r="F25" s="41"/>
+      <c r="G25" s="41"/>
       <c r="H25" s="32">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I25" s="32" t="s">
         <v>17</v>
@@ -8193,13 +8278,13 @@
         <v>3</v>
       </c>
       <c r="L25" s="33">
-        <v>0.125</v>
+        <v>0.14583333333333401</v>
       </c>
       <c r="M25" s="32" t="s">
         <v>14</v>
       </c>
       <c r="N25" s="32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="T25" s="1" t="b">
         <f t="shared" si="1"/>
@@ -8217,25 +8302,25 @@
       </c>
       <c r="AD25" s="1">
         <f>COUNTIF(Responsabilite,AC25)</f>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="AE25" s="19">
         <f>SUMIFS(Duree, Responsabilite,AC25)</f>
-        <v>0.34375000000000022</v>
+        <v>1.1770833333333304</v>
       </c>
     </row>
     <row r="26" spans="3:31" x14ac:dyDescent="0.3">
       <c r="C26" s="13">
         <v>11</v>
       </c>
-      <c r="D26" s="39" t="s">
-        <v>85</v>
-      </c>
-      <c r="E26" s="39"/>
-      <c r="F26" s="39"/>
-      <c r="G26" s="39"/>
+      <c r="D26" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="42"/>
       <c r="H26" s="34">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I26" s="34" t="s">
         <v>17</v>
@@ -8244,10 +8329,10 @@
         <v>3</v>
       </c>
       <c r="K26" s="34">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L26" s="35">
-        <v>8.3333333333333398E-2</v>
+        <v>0.22916666666666666</v>
       </c>
       <c r="M26" s="34" t="s">
         <v>14</v>
@@ -8271,25 +8356,25 @@
       </c>
       <c r="AD26" s="1">
         <f>COUNTIF(Responsabilite,AC26)</f>
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="AE26" s="19">
         <f>SUMIFS(Duree, Responsabilite,AC26)</f>
-        <v>0.44791666666666741</v>
+        <v>1.385416666666667</v>
       </c>
     </row>
     <row r="27" spans="3:31" x14ac:dyDescent="0.3">
       <c r="C27" s="12">
         <v>12</v>
       </c>
-      <c r="D27" s="42" t="s">
-        <v>81</v>
-      </c>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
+      <c r="D27" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="E27" s="41"/>
+      <c r="F27" s="41"/>
+      <c r="G27" s="41"/>
       <c r="H27" s="32">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I27" s="32" t="s">
         <v>17</v>
@@ -8298,16 +8383,16 @@
         <v>3</v>
       </c>
       <c r="K27" s="32">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L27" s="33">
-        <v>9.375E-2</v>
+        <v>8.3333333333333398E-2</v>
       </c>
       <c r="M27" s="32" t="s">
         <v>14</v>
       </c>
       <c r="N27" s="32" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="T27" s="1" t="b">
         <f t="shared" si="1"/>
@@ -8325,7 +8410,7 @@
       </c>
       <c r="AD27" s="1">
         <f>COUNTIF(Responsabilite,AC27)</f>
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="AE27" s="19">
         <f>SUMIFS(Duree, Responsabilite,AC27)</f>
@@ -8336,12 +8421,12 @@
       <c r="C28" s="13">
         <v>13</v>
       </c>
-      <c r="D28" s="39" t="s">
-        <v>82</v>
-      </c>
-      <c r="E28" s="39"/>
-      <c r="F28" s="39"/>
-      <c r="G28" s="39"/>
+      <c r="D28" s="42" t="s">
+        <v>80</v>
+      </c>
+      <c r="E28" s="42"/>
+      <c r="F28" s="42"/>
+      <c r="G28" s="42"/>
       <c r="H28" s="34">
         <v>8</v>
       </c>
@@ -8349,19 +8434,19 @@
         <v>17</v>
       </c>
       <c r="J28" s="34">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K28" s="34">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L28" s="35">
-        <v>8.3333333333333398E-2</v>
+        <v>0.16666666666666599</v>
       </c>
       <c r="M28" s="34" t="s">
         <v>14</v>
       </c>
       <c r="N28" s="34" t="s">
-        <v>21</v>
+        <v>73</v>
       </c>
       <c r="T28" s="1" t="b">
         <f>ISBLANK(D28)</f>
@@ -8379,7 +8464,7 @@
       </c>
       <c r="AD28" s="1">
         <f>COUNTIF(Responsabilite,AC28)</f>
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="AE28" s="19">
         <f>SUMIFS(Duree, Responsabilite,AC28)</f>
@@ -8390,23 +8475,23 @@
       <c r="C29" s="12">
         <v>14</v>
       </c>
-      <c r="D29" s="42" t="s">
-        <v>83</v>
-      </c>
-      <c r="E29" s="42"/>
-      <c r="F29" s="42"/>
-      <c r="G29" s="42"/>
+      <c r="D29" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="E29" s="41"/>
+      <c r="F29" s="41"/>
+      <c r="G29" s="41"/>
       <c r="H29" s="32">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="I29" s="32" t="s">
         <v>17</v>
       </c>
       <c r="J29" s="32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K29" s="32">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L29" s="33">
         <v>8.3333333333333398E-2</v>
@@ -8415,7 +8500,7 @@
         <v>14</v>
       </c>
       <c r="N29" s="32" t="s">
-        <v>21</v>
+        <v>73</v>
       </c>
       <c r="T29" s="1" t="b">
         <f>ISBLANK(D29)</f>
@@ -8432,12 +8517,12 @@
       <c r="C30" s="13">
         <v>15</v>
       </c>
-      <c r="D30" s="39" t="s">
-        <v>84</v>
-      </c>
-      <c r="E30" s="39"/>
-      <c r="F30" s="39"/>
-      <c r="G30" s="39"/>
+      <c r="D30" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="E30" s="42"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="42"/>
       <c r="H30" s="34">
         <v>13</v>
       </c>
@@ -8445,19 +8530,19 @@
         <v>17</v>
       </c>
       <c r="J30" s="34">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K30" s="34">
         <v>2</v>
       </c>
       <c r="L30" s="35">
-        <v>0.125</v>
+        <v>0.16666666666666599</v>
       </c>
       <c r="M30" s="34" t="s">
         <v>14</v>
       </c>
       <c r="N30" s="34" t="s">
-        <v>73</v>
+        <v>21</v>
       </c>
       <c r="T30" s="1" t="b">
         <f t="shared" si="1"/>
@@ -8480,20 +8565,36 @@
       <c r="C31" s="12">
         <v>16</v>
       </c>
-      <c r="D31" s="42"/>
-      <c r="E31" s="42"/>
-      <c r="F31" s="42"/>
-      <c r="G31" s="42"/>
-      <c r="H31" s="32"/>
-      <c r="I31" s="32"/>
-      <c r="J31" s="32"/>
-      <c r="K31" s="32"/>
-      <c r="L31" s="33"/>
-      <c r="M31" s="32"/>
-      <c r="N31" s="32"/>
+      <c r="D31" s="41" t="s">
+        <v>94</v>
+      </c>
+      <c r="E31" s="41"/>
+      <c r="F31" s="41"/>
+      <c r="G31" s="41"/>
+      <c r="H31" s="32">
+        <v>14</v>
+      </c>
+      <c r="I31" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="J31" s="32">
+        <v>2</v>
+      </c>
+      <c r="K31" s="32">
+        <v>3</v>
+      </c>
+      <c r="L31" s="33">
+        <v>0.16666666666666599</v>
+      </c>
+      <c r="M31" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="N31" s="32" t="s">
+        <v>21</v>
+      </c>
       <c r="T31" s="1" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U31" s="2">
         <v>15</v>
@@ -8506,31 +8607,47 @@
       </c>
       <c r="AD31" s="1">
         <f>COUNTIF(Categorie,AC31)</f>
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="AE31" s="19">
         <f>SUMIFS(Duree, Categorie,AC31)</f>
-        <v>2.8229166666627945</v>
+        <v>5.9479166666628061</v>
       </c>
     </row>
     <row r="32" spans="3:31" x14ac:dyDescent="0.3">
       <c r="C32" s="13">
         <v>17</v>
       </c>
-      <c r="D32" s="39"/>
-      <c r="E32" s="39"/>
-      <c r="F32" s="39"/>
-      <c r="G32" s="39"/>
-      <c r="H32" s="34"/>
-      <c r="I32" s="34"/>
-      <c r="J32" s="34"/>
-      <c r="K32" s="34"/>
-      <c r="L32" s="35"/>
-      <c r="M32" s="34"/>
-      <c r="N32" s="34"/>
+      <c r="D32" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="E32" s="42"/>
+      <c r="F32" s="42"/>
+      <c r="G32" s="42"/>
+      <c r="H32" s="34">
+        <v>14</v>
+      </c>
+      <c r="I32" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="J32" s="34">
+        <v>3</v>
+      </c>
+      <c r="K32" s="34">
+        <v>2</v>
+      </c>
+      <c r="L32" s="35">
+        <v>0.16666666666666599</v>
+      </c>
+      <c r="M32" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="N32" s="34" t="s">
+        <v>73</v>
+      </c>
       <c r="T32" s="1" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U32" s="2">
         <v>16</v>
@@ -8543,31 +8660,47 @@
       </c>
       <c r="AD32" s="1">
         <f>COUNTIF(Categorie,AC32)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AE32" s="19">
         <f>SUMIFS(Duree, Categorie,AC32)</f>
-        <v>0</v>
+        <v>0.22916666666666702</v>
       </c>
     </row>
     <row r="33" spans="3:31" x14ac:dyDescent="0.3">
       <c r="C33" s="12">
         <v>18</v>
       </c>
-      <c r="D33" s="42"/>
-      <c r="E33" s="42"/>
-      <c r="F33" s="42"/>
-      <c r="G33" s="42"/>
-      <c r="H33" s="32"/>
-      <c r="I33" s="32"/>
-      <c r="J33" s="32"/>
-      <c r="K33" s="32"/>
-      <c r="L33" s="33"/>
-      <c r="M33" s="32"/>
-      <c r="N33" s="32"/>
+      <c r="D33" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="E33" s="41"/>
+      <c r="F33" s="41"/>
+      <c r="G33" s="41"/>
+      <c r="H33" s="32">
+        <v>12</v>
+      </c>
+      <c r="I33" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="J33" s="32">
+        <v>2</v>
+      </c>
+      <c r="K33" s="32">
+        <v>1</v>
+      </c>
+      <c r="L33" s="33">
+        <v>0.16666666666666599</v>
+      </c>
+      <c r="M33" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="N33" s="32" t="s">
+        <v>74</v>
+      </c>
       <c r="T33" s="1" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U33" s="2">
         <v>17</v>
@@ -8580,31 +8713,47 @@
       </c>
       <c r="AD33" s="1">
         <f>COUNTIF(Categorie,AC33)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE33" s="19">
         <f>SUMIFS(Duree, Categorie,AC33)</f>
-        <v>0</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="34" spans="3:31" x14ac:dyDescent="0.3">
       <c r="C34" s="13">
         <v>19</v>
       </c>
-      <c r="D34" s="39"/>
-      <c r="E34" s="39"/>
-      <c r="F34" s="39"/>
-      <c r="G34" s="39"/>
-      <c r="H34" s="34"/>
-      <c r="I34" s="34"/>
-      <c r="J34" s="34"/>
-      <c r="K34" s="34"/>
-      <c r="L34" s="35"/>
-      <c r="M34" s="34"/>
-      <c r="N34" s="34"/>
+      <c r="D34" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="E34" s="42"/>
+      <c r="F34" s="42"/>
+      <c r="G34" s="42"/>
+      <c r="H34" s="34">
+        <v>12</v>
+      </c>
+      <c r="I34" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="J34" s="34">
+        <v>2</v>
+      </c>
+      <c r="K34" s="34">
+        <v>2</v>
+      </c>
+      <c r="L34" s="35">
+        <v>0.125</v>
+      </c>
+      <c r="M34" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="N34" s="34" t="s">
+        <v>73</v>
+      </c>
       <c r="T34" s="1" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U34" s="2">
         <v>18</v>
@@ -8617,20 +8766,36 @@
       <c r="C35" s="12">
         <v>20</v>
       </c>
-      <c r="D35" s="42"/>
-      <c r="E35" s="42"/>
-      <c r="F35" s="42"/>
-      <c r="G35" s="42"/>
-      <c r="H35" s="32"/>
-      <c r="I35" s="32"/>
-      <c r="J35" s="32"/>
-      <c r="K35" s="32"/>
-      <c r="L35" s="33"/>
-      <c r="M35" s="32"/>
-      <c r="N35" s="32"/>
+      <c r="D35" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="E35" s="41"/>
+      <c r="F35" s="41"/>
+      <c r="G35" s="41"/>
+      <c r="H35" s="32">
+        <v>12</v>
+      </c>
+      <c r="I35" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="J35" s="32">
+        <v>1</v>
+      </c>
+      <c r="K35" s="32">
+        <v>1</v>
+      </c>
+      <c r="L35" s="33">
+        <v>6.25E-2</v>
+      </c>
+      <c r="M35" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="N35" s="32" t="s">
+        <v>21</v>
+      </c>
       <c r="T35" s="1" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U35" s="2">
         <v>19</v>
@@ -8649,20 +8814,36 @@
       <c r="C36" s="13">
         <v>21</v>
       </c>
-      <c r="D36" s="39"/>
-      <c r="E36" s="39"/>
-      <c r="F36" s="39"/>
-      <c r="G36" s="39"/>
-      <c r="H36" s="34"/>
-      <c r="I36" s="34"/>
-      <c r="J36" s="34"/>
-      <c r="K36" s="34"/>
-      <c r="L36" s="35"/>
-      <c r="M36" s="34"/>
-      <c r="N36" s="34"/>
+      <c r="D36" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="E36" s="42"/>
+      <c r="F36" s="42"/>
+      <c r="G36" s="42"/>
+      <c r="H36" s="34">
+        <v>10</v>
+      </c>
+      <c r="I36" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="J36" s="34">
+        <v>2</v>
+      </c>
+      <c r="K36" s="34">
+        <v>3</v>
+      </c>
+      <c r="L36" s="35">
+        <v>0.125</v>
+      </c>
+      <c r="M36" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="N36" s="34" t="s">
+        <v>74</v>
+      </c>
       <c r="T36" s="1" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U36" s="2">
         <v>20</v>
@@ -8675,31 +8856,47 @@
       </c>
       <c r="AD36" s="1">
         <f>COUNTIF(Difficulte,W17)</f>
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="AE36" s="19">
         <f>SUMIFS(Duree, Difficulte,W17)</f>
-        <v>0.20833333333333345</v>
+        <v>1.3854166666666685</v>
       </c>
     </row>
     <row r="37" spans="3:31" x14ac:dyDescent="0.3">
       <c r="C37" s="12">
         <v>22</v>
       </c>
-      <c r="D37" s="42"/>
-      <c r="E37" s="42"/>
-      <c r="F37" s="42"/>
-      <c r="G37" s="42"/>
-      <c r="H37" s="32"/>
-      <c r="I37" s="32"/>
-      <c r="J37" s="32"/>
-      <c r="K37" s="32"/>
-      <c r="L37" s="33"/>
-      <c r="M37" s="32"/>
-      <c r="N37" s="32"/>
+      <c r="D37" s="41" t="s">
+        <v>93</v>
+      </c>
+      <c r="E37" s="41"/>
+      <c r="F37" s="41"/>
+      <c r="G37" s="41"/>
+      <c r="H37" s="32">
+        <v>9</v>
+      </c>
+      <c r="I37" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="J37" s="32">
+        <v>3</v>
+      </c>
+      <c r="K37" s="32">
+        <v>2</v>
+      </c>
+      <c r="L37" s="33">
+        <v>0.20833333333333001</v>
+      </c>
+      <c r="M37" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="N37" s="32" t="s">
+        <v>74</v>
+      </c>
       <c r="T37" s="1" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U37" s="2">
         <v>21</v>
@@ -8712,31 +8909,47 @@
       </c>
       <c r="AD37" s="1">
         <f>COUNTIF(Difficulte,W18)</f>
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="AE37" s="19">
         <f>SUMIFS(Duree, Difficulte,W18)</f>
-        <v>0.62500000000002309</v>
+        <v>2.1666666666666896</v>
       </c>
     </row>
     <row r="38" spans="3:31" x14ac:dyDescent="0.3">
       <c r="C38" s="13">
         <v>23</v>
       </c>
-      <c r="D38" s="39"/>
-      <c r="E38" s="39"/>
-      <c r="F38" s="39"/>
-      <c r="G38" s="39"/>
-      <c r="H38" s="34"/>
-      <c r="I38" s="34"/>
-      <c r="J38" s="34"/>
-      <c r="K38" s="34"/>
-      <c r="L38" s="35"/>
-      <c r="M38" s="34"/>
-      <c r="N38" s="34"/>
+      <c r="D38" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="E38" s="42"/>
+      <c r="F38" s="42"/>
+      <c r="G38" s="42"/>
+      <c r="H38" s="34">
+        <v>15</v>
+      </c>
+      <c r="I38" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="J38" s="34">
+        <v>2</v>
+      </c>
+      <c r="K38" s="34">
+        <v>2</v>
+      </c>
+      <c r="L38" s="35">
+        <v>8.3333333333333398E-2</v>
+      </c>
+      <c r="M38" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="N38" s="34" t="s">
+        <v>73</v>
+      </c>
       <c r="T38" s="1" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U38" s="2">
         <v>22</v>
@@ -8749,31 +8962,47 @@
       </c>
       <c r="AD38" s="1">
         <f>COUNTIF(Difficulte,W19)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AE38" s="19">
         <f>SUMIFS(Duree, Difficulte,W19)</f>
-        <v>1.9895833333294375</v>
+        <v>2.749999999996116</v>
       </c>
     </row>
     <row r="39" spans="3:31" x14ac:dyDescent="0.3">
       <c r="C39" s="12">
         <v>24</v>
       </c>
-      <c r="D39" s="42"/>
-      <c r="E39" s="42"/>
-      <c r="F39" s="42"/>
-      <c r="G39" s="42"/>
-      <c r="H39" s="32"/>
-      <c r="I39" s="32"/>
-      <c r="J39" s="32"/>
-      <c r="K39" s="32"/>
-      <c r="L39" s="33"/>
-      <c r="M39" s="32"/>
-      <c r="N39" s="32"/>
+      <c r="D39" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="E39" s="41"/>
+      <c r="F39" s="41"/>
+      <c r="G39" s="41"/>
+      <c r="H39" s="32">
+        <v>15</v>
+      </c>
+      <c r="I39" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="J39" s="32">
+        <v>2</v>
+      </c>
+      <c r="K39" s="32">
+        <v>2</v>
+      </c>
+      <c r="L39" s="33">
+        <v>6.25E-2</v>
+      </c>
+      <c r="M39" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="N39" s="32" t="s">
+        <v>21</v>
+      </c>
       <c r="T39" s="1" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U39" s="2">
         <v>23</v>
@@ -8786,20 +9015,36 @@
       <c r="C40" s="13">
         <v>25</v>
       </c>
-      <c r="D40" s="39"/>
-      <c r="E40" s="39"/>
-      <c r="F40" s="39"/>
-      <c r="G40" s="39"/>
-      <c r="H40" s="34"/>
-      <c r="I40" s="34"/>
-      <c r="J40" s="34"/>
-      <c r="K40" s="34"/>
-      <c r="L40" s="35"/>
-      <c r="M40" s="34"/>
-      <c r="N40" s="34"/>
+      <c r="D40" s="42" t="s">
+        <v>97</v>
+      </c>
+      <c r="E40" s="42"/>
+      <c r="F40" s="42"/>
+      <c r="G40" s="42"/>
+      <c r="H40" s="34">
+        <v>10</v>
+      </c>
+      <c r="I40" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="J40" s="34">
+        <v>2</v>
+      </c>
+      <c r="K40" s="34">
+        <v>2</v>
+      </c>
+      <c r="L40" s="35">
+        <v>0.14583333333333401</v>
+      </c>
+      <c r="M40" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="N40" s="34" t="s">
+        <v>21</v>
+      </c>
       <c r="T40" s="1" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U40" s="2">
         <v>24</v>
@@ -8818,20 +9063,36 @@
       <c r="C41" s="12">
         <v>26</v>
       </c>
-      <c r="D41" s="42"/>
-      <c r="E41" s="42"/>
-      <c r="F41" s="42"/>
-      <c r="G41" s="42"/>
-      <c r="H41" s="32"/>
-      <c r="I41" s="32"/>
-      <c r="J41" s="32"/>
-      <c r="K41" s="32"/>
-      <c r="L41" s="33"/>
-      <c r="M41" s="32"/>
-      <c r="N41" s="32"/>
+      <c r="D41" s="41" t="s">
+        <v>104</v>
+      </c>
+      <c r="E41" s="41"/>
+      <c r="F41" s="41"/>
+      <c r="G41" s="41"/>
+      <c r="H41" s="32">
+        <v>23</v>
+      </c>
+      <c r="I41" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="J41" s="32">
+        <v>3</v>
+      </c>
+      <c r="K41" s="32">
+        <v>3</v>
+      </c>
+      <c r="L41" s="33">
+        <v>0.33333333333335002</v>
+      </c>
+      <c r="M41" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="N41" s="32" t="s">
+        <v>21</v>
+      </c>
       <c r="T41" s="1" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U41" s="2">
         <v>25</v>
@@ -8844,31 +9105,47 @@
       </c>
       <c r="AD41" s="1">
         <f>COUNTIF(Incertitude,X17)</f>
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="AE41" s="19">
         <f>SUMIFS(Duree, Incertitude,X17)</f>
-        <v>0.54166666666668972</v>
+        <v>2.3437500000000249</v>
       </c>
     </row>
     <row r="42" spans="3:31" x14ac:dyDescent="0.3">
       <c r="C42" s="13">
         <v>27</v>
       </c>
-      <c r="D42" s="39"/>
-      <c r="E42" s="39"/>
-      <c r="F42" s="39"/>
-      <c r="G42" s="39"/>
-      <c r="H42" s="34"/>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
-      <c r="K42" s="34"/>
-      <c r="L42" s="35"/>
-      <c r="M42" s="34"/>
-      <c r="N42" s="34"/>
+      <c r="D42" s="42" t="s">
+        <v>101</v>
+      </c>
+      <c r="E42" s="42"/>
+      <c r="F42" s="42"/>
+      <c r="G42" s="42"/>
+      <c r="H42" s="34">
+        <v>10</v>
+      </c>
+      <c r="I42" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="J42" s="34">
+        <v>1</v>
+      </c>
+      <c r="K42" s="34">
+        <v>1</v>
+      </c>
+      <c r="L42" s="35">
+        <v>0.125</v>
+      </c>
+      <c r="M42" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="N42" s="34" t="s">
+        <v>21</v>
+      </c>
       <c r="T42" s="1" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U42" s="2">
         <v>26</v>
@@ -8881,31 +9158,47 @@
       </c>
       <c r="AD42" s="1">
         <f>COUNTIF(Incertitude,X18)</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="AE42" s="19">
         <f>SUMIFS(Duree, Incertitude,X18)</f>
-        <v>1.8333333333294373</v>
+        <v>2.6666666666627665</v>
       </c>
     </row>
     <row r="43" spans="3:31" x14ac:dyDescent="0.3">
       <c r="C43" s="12">
         <v>28</v>
       </c>
-      <c r="D43" s="42"/>
-      <c r="E43" s="42"/>
-      <c r="F43" s="42"/>
-      <c r="G43" s="42"/>
-      <c r="H43" s="32"/>
-      <c r="I43" s="32"/>
-      <c r="J43" s="32"/>
-      <c r="K43" s="32"/>
-      <c r="L43" s="33"/>
-      <c r="M43" s="32"/>
-      <c r="N43" s="32"/>
+      <c r="D43" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="E43" s="41"/>
+      <c r="F43" s="41"/>
+      <c r="G43" s="41"/>
+      <c r="H43" s="32">
+        <v>10</v>
+      </c>
+      <c r="I43" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="J43" s="32">
+        <v>1</v>
+      </c>
+      <c r="K43" s="32">
+        <v>1</v>
+      </c>
+      <c r="L43" s="33">
+        <v>0.13541666666666699</v>
+      </c>
+      <c r="M43" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="N43" s="32" t="s">
+        <v>73</v>
+      </c>
       <c r="T43" s="1" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U43" s="2">
         <v>27</v>
@@ -8918,31 +9211,47 @@
       </c>
       <c r="AD43" s="1">
         <f>COUNTIF(Incertitude,X19)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="AE43" s="19">
         <f>SUMIFS(Duree, Incertitude,X19)</f>
-        <v>0.44791666666666741</v>
+        <v>1.2916666666666825</v>
       </c>
     </row>
     <row r="44" spans="3:31" x14ac:dyDescent="0.3">
       <c r="C44" s="13">
         <v>29</v>
       </c>
-      <c r="D44" s="39"/>
-      <c r="E44" s="39"/>
-      <c r="F44" s="39"/>
-      <c r="G44" s="39"/>
-      <c r="H44" s="34"/>
-      <c r="I44" s="34"/>
-      <c r="J44" s="34"/>
-      <c r="K44" s="34"/>
-      <c r="L44" s="35"/>
-      <c r="M44" s="34"/>
-      <c r="N44" s="34"/>
+      <c r="D44" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="E44" s="42"/>
+      <c r="F44" s="42"/>
+      <c r="G44" s="42"/>
+      <c r="H44" s="34">
+        <v>20</v>
+      </c>
+      <c r="I44" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="J44" s="34">
+        <v>1</v>
+      </c>
+      <c r="K44" s="34">
+        <v>1</v>
+      </c>
+      <c r="L44" s="35">
+        <v>0.125</v>
+      </c>
+      <c r="M44" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="N44" s="34" t="s">
+        <v>73</v>
+      </c>
       <c r="T44" s="1" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U44" s="2">
         <v>28</v>
@@ -8955,20 +9264,36 @@
       <c r="C45" s="12">
         <v>30</v>
       </c>
-      <c r="D45" s="42"/>
-      <c r="E45" s="42"/>
-      <c r="F45" s="42"/>
-      <c r="G45" s="42"/>
-      <c r="H45" s="32"/>
-      <c r="I45" s="32"/>
-      <c r="J45" s="32"/>
-      <c r="K45" s="32"/>
-      <c r="L45" s="33"/>
-      <c r="M45" s="32"/>
-      <c r="N45" s="32"/>
+      <c r="D45" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="E45" s="41"/>
+      <c r="F45" s="41"/>
+      <c r="G45" s="41"/>
+      <c r="H45" s="32">
+        <v>12</v>
+      </c>
+      <c r="I45" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="J45" s="32">
+        <v>1</v>
+      </c>
+      <c r="K45" s="32">
+        <v>1</v>
+      </c>
+      <c r="L45" s="33">
+        <v>0.14583333333333401</v>
+      </c>
+      <c r="M45" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="N45" s="32" t="s">
+        <v>74</v>
+      </c>
       <c r="T45" s="1" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U45" s="2">
         <v>29</v>
@@ -8981,20 +9306,36 @@
       <c r="C46" s="13">
         <v>31</v>
       </c>
-      <c r="D46" s="39"/>
-      <c r="E46" s="39"/>
-      <c r="F46" s="39"/>
-      <c r="G46" s="39"/>
-      <c r="H46" s="34"/>
-      <c r="I46" s="34"/>
-      <c r="J46" s="34"/>
-      <c r="K46" s="34"/>
-      <c r="L46" s="35"/>
-      <c r="M46" s="34"/>
-      <c r="N46" s="34"/>
+      <c r="D46" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="E46" s="42"/>
+      <c r="F46" s="42"/>
+      <c r="G46" s="42"/>
+      <c r="H46" s="34">
+        <v>20</v>
+      </c>
+      <c r="I46" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="J46" s="34">
+        <v>2</v>
+      </c>
+      <c r="K46" s="34">
+        <v>1</v>
+      </c>
+      <c r="L46" s="35">
+        <v>8.3333333333333398E-2</v>
+      </c>
+      <c r="M46" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="N46" s="34" t="s">
+        <v>21</v>
+      </c>
       <c r="T46" s="1" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>ISBLANK(D46)</f>
+        <v>0</v>
       </c>
       <c r="U46" s="2">
         <v>30</v>
@@ -9007,20 +9348,36 @@
       <c r="C47" s="12">
         <v>32</v>
       </c>
-      <c r="D47" s="42"/>
-      <c r="E47" s="42"/>
-      <c r="F47" s="42"/>
-      <c r="G47" s="42"/>
-      <c r="H47" s="32"/>
-      <c r="I47" s="32"/>
-      <c r="J47" s="32"/>
-      <c r="K47" s="32"/>
-      <c r="L47" s="33"/>
-      <c r="M47" s="32"/>
-      <c r="N47" s="32"/>
+      <c r="D47" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="E47" s="39"/>
+      <c r="F47" s="39"/>
+      <c r="G47" s="39"/>
+      <c r="H47" s="32">
+        <v>22</v>
+      </c>
+      <c r="I47" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="J47" s="32">
+        <v>2</v>
+      </c>
+      <c r="K47" s="32">
+        <v>2</v>
+      </c>
+      <c r="L47" s="33">
+        <v>8.3333333333333398E-2</v>
+      </c>
+      <c r="M47" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="N47" s="32" t="s">
+        <v>21</v>
+      </c>
       <c r="T47" s="1" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U47" s="2">
         <v>31</v>
@@ -9033,20 +9390,36 @@
       <c r="C48" s="13">
         <v>33</v>
       </c>
-      <c r="D48" s="39"/>
-      <c r="E48" s="39"/>
-      <c r="F48" s="39"/>
-      <c r="G48" s="39"/>
-      <c r="H48" s="34"/>
-      <c r="I48" s="34"/>
-      <c r="J48" s="34"/>
-      <c r="K48" s="34"/>
-      <c r="L48" s="35"/>
-      <c r="M48" s="34"/>
-      <c r="N48" s="34"/>
+      <c r="D48" s="42" t="s">
+        <v>102</v>
+      </c>
+      <c r="E48" s="42"/>
+      <c r="F48" s="42"/>
+      <c r="G48" s="42"/>
+      <c r="H48" s="34">
+        <v>19</v>
+      </c>
+      <c r="I48" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="J48" s="34">
+        <v>1</v>
+      </c>
+      <c r="K48" s="34">
+        <v>1</v>
+      </c>
+      <c r="L48" s="35">
+        <v>0.125</v>
+      </c>
+      <c r="M48" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="N48" s="34" t="s">
+        <v>73</v>
+      </c>
       <c r="T48" s="1" t="b">
         <f t="shared" ref="T48:T65" si="4">ISBLANK(D48)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U48" s="2">
         <v>32</v>
@@ -9059,20 +9432,36 @@
       <c r="C49" s="12">
         <v>34</v>
       </c>
-      <c r="D49" s="42"/>
-      <c r="E49" s="42"/>
-      <c r="F49" s="42"/>
-      <c r="G49" s="42"/>
-      <c r="H49" s="32"/>
-      <c r="I49" s="32"/>
-      <c r="J49" s="32"/>
-      <c r="K49" s="32"/>
-      <c r="L49" s="33"/>
-      <c r="M49" s="32"/>
-      <c r="N49" s="32"/>
+      <c r="D49" s="41" t="s">
+        <v>106</v>
+      </c>
+      <c r="E49" s="41"/>
+      <c r="F49" s="41"/>
+      <c r="G49" s="41"/>
+      <c r="H49" s="32">
+        <v>16</v>
+      </c>
+      <c r="I49" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="J49" s="32">
+        <v>2</v>
+      </c>
+      <c r="K49" s="32">
+        <v>1</v>
+      </c>
+      <c r="L49" s="33">
+        <v>0.125</v>
+      </c>
+      <c r="M49" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="N49" s="32" t="s">
+        <v>21</v>
+      </c>
       <c r="T49" s="1" t="b">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U49" s="2">
         <v>33</v>
@@ -9088,20 +9477,36 @@
       <c r="C50" s="13">
         <v>35</v>
       </c>
-      <c r="D50" s="39"/>
-      <c r="E50" s="39"/>
-      <c r="F50" s="39"/>
-      <c r="G50" s="39"/>
-      <c r="H50" s="34"/>
-      <c r="I50" s="34"/>
-      <c r="J50" s="34"/>
-      <c r="K50" s="34"/>
-      <c r="L50" s="35"/>
-      <c r="M50" s="34"/>
-      <c r="N50" s="34"/>
+      <c r="D50" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="E50" s="42"/>
+      <c r="F50" s="42"/>
+      <c r="G50" s="42"/>
+      <c r="H50" s="34">
+        <v>10</v>
+      </c>
+      <c r="I50" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="J50" s="34">
+        <v>2</v>
+      </c>
+      <c r="K50" s="34">
+        <v>1</v>
+      </c>
+      <c r="L50" s="35">
+        <v>0.14583333333333401</v>
+      </c>
+      <c r="M50" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="N50" s="34" t="s">
+        <v>73</v>
+      </c>
       <c r="T50" s="1" t="b">
-        <f t="shared" si="4"/>
-        <v>1</v>
+        <f>ISBLANK(D50)</f>
+        <v>0</v>
       </c>
       <c r="U50" s="2">
         <v>34</v>
@@ -9117,20 +9522,36 @@
       <c r="C51" s="12">
         <v>36</v>
       </c>
-      <c r="D51" s="42"/>
-      <c r="E51" s="42"/>
-      <c r="F51" s="42"/>
-      <c r="G51" s="42"/>
-      <c r="H51" s="32"/>
-      <c r="I51" s="32"/>
-      <c r="J51" s="32"/>
-      <c r="K51" s="32"/>
-      <c r="L51" s="33"/>
-      <c r="M51" s="32"/>
-      <c r="N51" s="32"/>
+      <c r="D51" s="41" t="s">
+        <v>112</v>
+      </c>
+      <c r="E51" s="41"/>
+      <c r="F51" s="41"/>
+      <c r="G51" s="41"/>
+      <c r="H51" s="32">
+        <v>25</v>
+      </c>
+      <c r="I51" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="J51" s="32">
+        <v>1</v>
+      </c>
+      <c r="K51" s="32">
+        <v>1</v>
+      </c>
+      <c r="L51" s="33">
+        <v>8.3333333333333398E-2</v>
+      </c>
+      <c r="M51" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="N51" s="32" t="s">
+        <v>74</v>
+      </c>
       <c r="T51" s="1" t="b">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U51" s="2">
         <v>35</v>
@@ -9146,10 +9567,10 @@
       <c r="C52" s="13">
         <v>37</v>
       </c>
-      <c r="D52" s="39"/>
-      <c r="E52" s="39"/>
-      <c r="F52" s="39"/>
-      <c r="G52" s="39"/>
+      <c r="D52" s="42"/>
+      <c r="E52" s="42"/>
+      <c r="F52" s="42"/>
+      <c r="G52" s="42"/>
       <c r="H52" s="34"/>
       <c r="I52" s="34"/>
       <c r="J52" s="34"/>
@@ -9175,10 +9596,10 @@
       <c r="C53" s="12">
         <v>38</v>
       </c>
-      <c r="D53" s="42"/>
-      <c r="E53" s="42"/>
-      <c r="F53" s="42"/>
-      <c r="G53" s="42"/>
+      <c r="D53" s="41"/>
+      <c r="E53" s="41"/>
+      <c r="F53" s="41"/>
+      <c r="G53" s="41"/>
       <c r="H53" s="32"/>
       <c r="I53" s="32"/>
       <c r="J53" s="32"/>
@@ -9204,10 +9625,10 @@
       <c r="C54" s="13">
         <v>39</v>
       </c>
-      <c r="D54" s="39"/>
-      <c r="E54" s="39"/>
-      <c r="F54" s="39"/>
-      <c r="G54" s="39"/>
+      <c r="D54" s="42"/>
+      <c r="E54" s="42"/>
+      <c r="F54" s="42"/>
+      <c r="G54" s="42"/>
       <c r="H54" s="34"/>
       <c r="I54" s="34"/>
       <c r="J54" s="34"/>
@@ -9233,20 +9654,34 @@
       <c r="C55" s="12">
         <v>40</v>
       </c>
-      <c r="D55" s="42"/>
-      <c r="E55" s="42"/>
-      <c r="F55" s="42"/>
-      <c r="G55" s="42"/>
+      <c r="D55" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="E55" s="41"/>
+      <c r="F55" s="41"/>
+      <c r="G55" s="41"/>
       <c r="H55" s="32"/>
-      <c r="I55" s="32"/>
-      <c r="J55" s="32"/>
-      <c r="K55" s="32"/>
-      <c r="L55" s="33"/>
-      <c r="M55" s="32"/>
-      <c r="N55" s="32"/>
+      <c r="I55" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="J55" s="32">
+        <v>2</v>
+      </c>
+      <c r="K55" s="32">
+        <v>1</v>
+      </c>
+      <c r="L55" s="33">
+        <v>0.104166666666667</v>
+      </c>
+      <c r="M55" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="N55" s="32" t="s">
+        <v>21</v>
+      </c>
       <c r="T55" s="1" t="b">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U55" s="2">
         <v>39</v>
@@ -9262,20 +9697,34 @@
       <c r="C56" s="13">
         <v>41</v>
       </c>
-      <c r="D56" s="39"/>
-      <c r="E56" s="39"/>
-      <c r="F56" s="39"/>
-      <c r="G56" s="39"/>
+      <c r="D56" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="E56" s="42"/>
+      <c r="F56" s="42"/>
+      <c r="G56" s="42"/>
       <c r="H56" s="34"/>
-      <c r="I56" s="34"/>
-      <c r="J56" s="34"/>
-      <c r="K56" s="34"/>
-      <c r="L56" s="35"/>
-      <c r="M56" s="34"/>
-      <c r="N56" s="34"/>
+      <c r="I56" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="J56" s="34">
+        <v>1</v>
+      </c>
+      <c r="K56" s="34">
+        <v>1</v>
+      </c>
+      <c r="L56" s="35">
+        <v>0.104166666666667</v>
+      </c>
+      <c r="M56" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="N56" s="34" t="s">
+        <v>21</v>
+      </c>
       <c r="T56" s="1" t="b">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U56" s="2">
         <v>40</v>
@@ -9291,10 +9740,10 @@
       <c r="C57" s="12">
         <v>42</v>
       </c>
-      <c r="D57" s="42"/>
-      <c r="E57" s="42"/>
-      <c r="F57" s="42"/>
-      <c r="G57" s="42"/>
+      <c r="D57" s="41"/>
+      <c r="E57" s="41"/>
+      <c r="F57" s="41"/>
+      <c r="G57" s="41"/>
       <c r="H57" s="32"/>
       <c r="I57" s="32"/>
       <c r="J57" s="32"/>
@@ -9320,20 +9769,34 @@
       <c r="C58" s="13">
         <v>43</v>
       </c>
-      <c r="D58" s="39"/>
-      <c r="E58" s="39"/>
-      <c r="F58" s="39"/>
-      <c r="G58" s="39"/>
+      <c r="D58" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="E58" s="42"/>
+      <c r="F58" s="42"/>
+      <c r="G58" s="42"/>
       <c r="H58" s="34"/>
-      <c r="I58" s="34"/>
-      <c r="J58" s="34"/>
-      <c r="K58" s="34"/>
-      <c r="L58" s="35"/>
-      <c r="M58" s="34"/>
-      <c r="N58" s="34"/>
+      <c r="I58" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="J58" s="34">
+        <v>2</v>
+      </c>
+      <c r="K58" s="34">
+        <v>3</v>
+      </c>
+      <c r="L58" s="35">
+        <v>0.125</v>
+      </c>
+      <c r="M58" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="N58" s="34" t="s">
+        <v>21</v>
+      </c>
       <c r="T58" s="1" t="b">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U58" s="2">
         <v>42</v>
@@ -9349,10 +9812,10 @@
       <c r="C59" s="12">
         <v>44</v>
       </c>
-      <c r="D59" s="42"/>
-      <c r="E59" s="42"/>
-      <c r="F59" s="42"/>
-      <c r="G59" s="42"/>
+      <c r="D59" s="41"/>
+      <c r="E59" s="41"/>
+      <c r="F59" s="41"/>
+      <c r="G59" s="41"/>
       <c r="H59" s="32"/>
       <c r="I59" s="32"/>
       <c r="J59" s="32"/>
@@ -9378,10 +9841,10 @@
       <c r="C60" s="13">
         <v>45</v>
       </c>
-      <c r="D60" s="39"/>
-      <c r="E60" s="39"/>
-      <c r="F60" s="39"/>
-      <c r="G60" s="39"/>
+      <c r="D60" s="42"/>
+      <c r="E60" s="42"/>
+      <c r="F60" s="42"/>
+      <c r="G60" s="42"/>
       <c r="H60" s="34"/>
       <c r="I60" s="34"/>
       <c r="J60" s="34"/>
@@ -9407,20 +9870,34 @@
       <c r="C61" s="12">
         <v>46</v>
       </c>
-      <c r="D61" s="42"/>
-      <c r="E61" s="42"/>
-      <c r="F61" s="42"/>
-      <c r="G61" s="42"/>
+      <c r="D61" s="41" t="s">
+        <v>108</v>
+      </c>
+      <c r="E61" s="41"/>
+      <c r="F61" s="41"/>
+      <c r="G61" s="41"/>
       <c r="H61" s="32"/>
-      <c r="I61" s="32"/>
-      <c r="J61" s="32"/>
-      <c r="K61" s="32"/>
-      <c r="L61" s="33"/>
-      <c r="M61" s="32"/>
-      <c r="N61" s="32"/>
+      <c r="I61" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="J61" s="32">
+        <v>1</v>
+      </c>
+      <c r="K61" s="32">
+        <v>1</v>
+      </c>
+      <c r="L61" s="33">
+        <v>8.3333333333333398E-2</v>
+      </c>
+      <c r="M61" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="N61" s="32" t="s">
+        <v>21</v>
+      </c>
       <c r="T61" s="1" t="b">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U61" s="2">
         <v>45</v>
@@ -9436,20 +9913,34 @@
       <c r="C62" s="13">
         <v>47</v>
       </c>
-      <c r="D62" s="39"/>
-      <c r="E62" s="39"/>
-      <c r="F62" s="39"/>
-      <c r="G62" s="39"/>
+      <c r="D62" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="E62" s="42"/>
+      <c r="F62" s="42"/>
+      <c r="G62" s="42"/>
       <c r="H62" s="34"/>
-      <c r="I62" s="34"/>
-      <c r="J62" s="34"/>
-      <c r="K62" s="34"/>
-      <c r="L62" s="35"/>
-      <c r="M62" s="34"/>
-      <c r="N62" s="34"/>
+      <c r="I62" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="J62" s="34">
+        <v>1</v>
+      </c>
+      <c r="K62" s="34">
+        <v>1</v>
+      </c>
+      <c r="L62" s="35">
+        <v>3.125E-2</v>
+      </c>
+      <c r="M62" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="N62" s="34" t="s">
+        <v>21</v>
+      </c>
       <c r="T62" s="1" t="b">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U62" s="2">
         <v>46</v>
@@ -9465,20 +9956,34 @@
       <c r="C63" s="12">
         <v>48</v>
       </c>
-      <c r="D63" s="42"/>
-      <c r="E63" s="42"/>
-      <c r="F63" s="42"/>
-      <c r="G63" s="42"/>
+      <c r="D63" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="E63" s="41"/>
+      <c r="F63" s="41"/>
+      <c r="G63" s="41"/>
       <c r="H63" s="32"/>
-      <c r="I63" s="32"/>
-      <c r="J63" s="32"/>
-      <c r="K63" s="32"/>
-      <c r="L63" s="33"/>
-      <c r="M63" s="32"/>
-      <c r="N63" s="32"/>
+      <c r="I63" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="J63" s="32">
+        <v>1</v>
+      </c>
+      <c r="K63" s="32">
+        <v>1</v>
+      </c>
+      <c r="L63" s="33">
+        <v>4.1666666666666699E-2</v>
+      </c>
+      <c r="M63" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="N63" s="32" t="s">
+        <v>21</v>
+      </c>
       <c r="T63" s="1" t="b">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U63" s="2">
         <v>47</v>
@@ -9494,10 +9999,10 @@
       <c r="C64" s="13">
         <v>49</v>
       </c>
-      <c r="D64" s="39"/>
-      <c r="E64" s="39"/>
-      <c r="F64" s="39"/>
-      <c r="G64" s="39"/>
+      <c r="D64" s="42"/>
+      <c r="E64" s="42"/>
+      <c r="F64" s="42"/>
+      <c r="G64" s="42"/>
       <c r="H64" s="34"/>
       <c r="I64" s="34"/>
       <c r="J64" s="34"/>
@@ -9579,7 +10084,7 @@
     <row r="68" spans="3:25" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="D68" s="1">
         <f>COUNTA(D16:D65)</f>
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="H68" s="2"/>
       <c r="I68" s="2"/>
@@ -9587,7 +10092,7 @@
       <c r="K68" s="2"/>
       <c r="L68" s="9">
         <f>SUM(L16:L65)</f>
-        <v>2.8229166666627945</v>
+        <v>6.302083333329473</v>
       </c>
       <c r="M68" s="2"/>
       <c r="N68" s="2"/>
@@ -9865,7 +10370,45 @@
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="tjqSiT+XspradLJBNpu0viI4TokIDIF0O7QeXm3BTZLmeAfSOw5TlniSFfStQ9LXJLtK7gLyf3B6jINr+qJ+Cg==" saltValue="/wSmyHkNAfBsPbW8NILu1w==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
-  <mergeCells count="55">
+  <mergeCells count="54">
+    <mergeCell ref="D20:G20"/>
+    <mergeCell ref="D15:G15"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="D19:G19"/>
+    <mergeCell ref="D32:G32"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="D21:G21"/>
+    <mergeCell ref="D24:G24"/>
+    <mergeCell ref="D25:G25"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="D28:G28"/>
+    <mergeCell ref="D29:G29"/>
+    <mergeCell ref="D30:G30"/>
+    <mergeCell ref="D31:G31"/>
+    <mergeCell ref="D44:G44"/>
+    <mergeCell ref="D33:G33"/>
+    <mergeCell ref="D34:G34"/>
+    <mergeCell ref="D35:G35"/>
+    <mergeCell ref="D36:G36"/>
+    <mergeCell ref="D37:G37"/>
+    <mergeCell ref="D38:G38"/>
+    <mergeCell ref="D39:G39"/>
+    <mergeCell ref="D40:G40"/>
+    <mergeCell ref="D41:G41"/>
+    <mergeCell ref="D42:G42"/>
+    <mergeCell ref="D43:G43"/>
+    <mergeCell ref="D53:G53"/>
+    <mergeCell ref="D54:G54"/>
+    <mergeCell ref="D55:G55"/>
+    <mergeCell ref="D56:G56"/>
+    <mergeCell ref="D45:G45"/>
+    <mergeCell ref="D46:G46"/>
+    <mergeCell ref="D48:G48"/>
+    <mergeCell ref="D49:G49"/>
+    <mergeCell ref="D50:G50"/>
     <mergeCell ref="D63:G63"/>
     <mergeCell ref="D64:G64"/>
     <mergeCell ref="D65:G65"/>
@@ -9882,45 +10425,6 @@
     <mergeCell ref="D62:G62"/>
     <mergeCell ref="D51:G51"/>
     <mergeCell ref="D52:G52"/>
-    <mergeCell ref="D53:G53"/>
-    <mergeCell ref="D54:G54"/>
-    <mergeCell ref="D55:G55"/>
-    <mergeCell ref="D56:G56"/>
-    <mergeCell ref="D45:G45"/>
-    <mergeCell ref="D46:G46"/>
-    <mergeCell ref="D47:G47"/>
-    <mergeCell ref="D48:G48"/>
-    <mergeCell ref="D49:G49"/>
-    <mergeCell ref="D50:G50"/>
-    <mergeCell ref="D44:G44"/>
-    <mergeCell ref="D33:G33"/>
-    <mergeCell ref="D34:G34"/>
-    <mergeCell ref="D35:G35"/>
-    <mergeCell ref="D36:G36"/>
-    <mergeCell ref="D37:G37"/>
-    <mergeCell ref="D38:G38"/>
-    <mergeCell ref="D39:G39"/>
-    <mergeCell ref="D40:G40"/>
-    <mergeCell ref="D41:G41"/>
-    <mergeCell ref="D42:G42"/>
-    <mergeCell ref="D43:G43"/>
-    <mergeCell ref="D32:G32"/>
-    <mergeCell ref="D22:G22"/>
-    <mergeCell ref="D21:G21"/>
-    <mergeCell ref="D24:G24"/>
-    <mergeCell ref="D25:G25"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="D28:G28"/>
-    <mergeCell ref="D29:G29"/>
-    <mergeCell ref="D30:G30"/>
-    <mergeCell ref="D31:G31"/>
-    <mergeCell ref="D20:G20"/>
-    <mergeCell ref="D15:G15"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="D18:G18"/>
-    <mergeCell ref="D19:G19"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:N2">
     <cfRule type="expression" dxfId="9" priority="3">
@@ -9978,7 +10482,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="8">
+  <dataValidations xWindow="1629" yWindow="1417" count="8">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Catégorie de la tâche" prompt="_x000a_Veuillez saisir la catégorie de la tâche._x000a__x000a_Essentielle -&gt; obligatoire_x000a_Souhaitable -&gt; envisagée_x000a_Optionnelle -&gt; facultative" sqref="I16:I65" xr:uid="{DD0CD761-E4CE-42EA-98B7-B4FB43663207}">
       <formula1>ListeCategorie</formula1>
     </dataValidation>
@@ -10033,7 +10537,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11C8C552-AE5F-48A4-9B18-A93F0BCBDB63}">
   <dimension ref="B1:M10"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="A2" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -10083,19 +10587,19 @@
       </c>
       <c r="D5" s="8">
         <f>COUNTIF(Sprint,D4)</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E5" s="8">
         <f>COUNTIF(Sprint,E4)</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F5" s="8">
         <f>COUNTIF(Sprint,F4)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G5" s="25">
         <f>SUM(C5:F5)</f>
-        <v>15</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.35">
@@ -10108,36 +10612,36 @@
       </c>
       <c r="D6" s="10">
         <f>SUMIFS(Duree, Sprint,D4)</f>
-        <v>0.95833333333333437</v>
+        <v>1.7499999999999978</v>
       </c>
       <c r="E6" s="10">
         <f>SUMIFS(Duree, Sprint,E4)</f>
-        <v>0</v>
+        <v>1.7187500000000153</v>
       </c>
       <c r="F6" s="10">
         <f>SUMIFS(Duree, Sprint,F4)</f>
-        <v>0</v>
+        <v>0.96875000000000144</v>
       </c>
       <c r="G6" s="26">
         <f>SUM(C6:F6)</f>
-        <v>2.8229166666627941</v>
+        <v>6.3020833333294748</v>
       </c>
     </row>
     <row r="9" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="48" t="s">
+      <c r="B9" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="48"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="48"/>
-      <c r="J9" s="48"/>
-      <c r="K9" s="48"/>
-      <c r="L9" s="48"/>
-      <c r="M9" s="48"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="50"/>
+      <c r="I9" s="50"/>
+      <c r="J9" s="50"/>
+      <c r="K9" s="50"/>
+      <c r="L9" s="50"/>
+      <c r="M9" s="50"/>
     </row>
     <row r="10" spans="2:13" ht="10.75" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
@@ -10167,25 +10671,25 @@
   <sheetData>
     <row r="1" spans="2:18" ht="13.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:18" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
-      <c r="M2" s="48"/>
-      <c r="N2" s="48"/>
-      <c r="O2" s="48"/>
-      <c r="P2" s="48"/>
-      <c r="Q2" s="48"/>
-      <c r="R2" s="48"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="50"/>
+      <c r="N2" s="50"/>
+      <c r="O2" s="50"/>
+      <c r="P2" s="50"/>
+      <c r="Q2" s="50"/>
+      <c r="R2" s="50"/>
     </row>
     <row r="3" spans="2:18" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:18" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
UPDATE planification ajout vue index
</commit_message>
<xml_diff>
--- a/docs/C61 - Sprint1c - Outil de planification.xlsx
+++ b/docs/C61 - Sprint1c - Outil de planification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GENES\Documents\School\GreenFlag\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44FAE404-520C-4C4A-BB34-C6259DD59E5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15BE01F0-E5FB-4426-8748-8A4EA10DD25A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -383,7 +383,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="114">
   <si>
     <t>Planification</t>
   </si>
@@ -848,6 +848,9 @@
   </si>
   <si>
     <t xml:space="preserve">Pages de confirmation email, page de menu (settings) </t>
+  </si>
+  <si>
+    <t>Creation des vues et indexs dans la base de donnée</t>
   </si>
 </sst>
 </file>
@@ -1727,7 +1730,7 @@
                   <c:v>1.8645833333294597</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.7499999999999978</c:v>
+                  <c:v>1.8333333333333313</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.7187500000000153</c:v>
@@ -2130,10 +2133,10 @@
                 <c:formatCode>[hh]:mm</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>15</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.7499999999999978</c:v>
+                  <c:v>1.8333333333333313</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2702,10 +2705,10 @@
                 <c:formatCode>[hh]:mm</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>39</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.9479166666628061</c:v>
+                  <c:v>6.0312499999961391</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3214,10 +3217,10 @@
                 <c:formatCode>[hh]:mm</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>16</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.1666666666666896</c:v>
+                  <c:v>2.2500000000000231</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3608,10 +3611,10 @@
                 <c:formatCode>[hh]:mm</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>23</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.3437500000000249</c:v>
+                  <c:v>2.4270833333333579</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7501,8 +7504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AF97"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A21" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53:G53"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61:G61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.28515625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -7676,7 +7679,7 @@
       <c r="N13" s="47"/>
       <c r="U13" s="2">
         <f>D68</f>
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AA13" s="2">
         <f>N7</f>
@@ -7919,11 +7922,11 @@
       </c>
       <c r="AD18" s="1">
         <f>COUNTIF(Sprint,AC18)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AE18" s="19">
         <f>SUMIFS(Duree, Sprint,AC18)</f>
-        <v>1.7499999999999978</v>
+        <v>1.8333333333333313</v>
       </c>
     </row>
     <row r="19" spans="3:31" x14ac:dyDescent="0.2">
@@ -8244,11 +8247,11 @@
       </c>
       <c r="AD24" s="1">
         <f>COUNTIF(Responsabilite,AC24)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="AE24" s="19">
         <f>SUMIFS(Duree, Responsabilite,AC24)</f>
-        <v>3.7395833333294766</v>
+        <v>3.82291666666281</v>
       </c>
     </row>
     <row r="25" spans="3:31" x14ac:dyDescent="0.2">
@@ -8406,7 +8409,7 @@
       </c>
       <c r="AD27" s="1">
         <f>COUNTIF(Responsabilite,AC27)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AE27" s="19">
         <f>SUMIFS(Duree, Responsabilite,AC27)</f>
@@ -8460,7 +8463,7 @@
       </c>
       <c r="AD28" s="1">
         <f>COUNTIF(Responsabilite,AC28)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AE28" s="19">
         <f>SUMIFS(Duree, Responsabilite,AC28)</f>
@@ -8603,11 +8606,11 @@
       </c>
       <c r="AD31" s="1">
         <f>COUNTIF(Categorie,AC31)</f>
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AE31" s="19">
         <f>SUMIFS(Duree, Categorie,AC31)</f>
-        <v>5.9479166666628061</v>
+        <v>6.0312499999961391</v>
       </c>
     </row>
     <row r="32" spans="3:31" x14ac:dyDescent="0.2">
@@ -8763,28 +8766,28 @@
         <v>20</v>
       </c>
       <c r="D35" s="43" t="s">
-        <v>83</v>
+        <v>113</v>
       </c>
       <c r="E35" s="43"/>
       <c r="F35" s="43"/>
       <c r="G35" s="43"/>
       <c r="H35" s="32">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="I35" s="32" t="s">
         <v>17</v>
       </c>
       <c r="J35" s="32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K35" s="32">
         <v>1</v>
       </c>
       <c r="L35" s="33">
-        <v>6.25E-2</v>
+        <v>8.3333333333333398E-2</v>
       </c>
       <c r="M35" s="32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N35" s="32" t="s">
         <v>21</v>
@@ -8811,31 +8814,31 @@
         <v>21</v>
       </c>
       <c r="D36" s="40" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E36" s="40"/>
       <c r="F36" s="40"/>
       <c r="G36" s="40"/>
       <c r="H36" s="34">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I36" s="34" t="s">
         <v>17</v>
       </c>
       <c r="J36" s="34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K36" s="34">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L36" s="35">
-        <v>0.125</v>
+        <v>6.25E-2</v>
       </c>
       <c r="M36" s="34" t="s">
         <v>15</v>
       </c>
       <c r="N36" s="34" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="T36" s="1" t="b">
         <f t="shared" si="1"/>
@@ -8864,25 +8867,25 @@
         <v>22</v>
       </c>
       <c r="D37" s="43" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="E37" s="43"/>
       <c r="F37" s="43"/>
       <c r="G37" s="43"/>
       <c r="H37" s="32">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I37" s="32" t="s">
         <v>17</v>
       </c>
       <c r="J37" s="32">
+        <v>2</v>
+      </c>
+      <c r="K37" s="32">
         <v>3</v>
       </c>
-      <c r="K37" s="32">
-        <v>2</v>
-      </c>
       <c r="L37" s="33">
-        <v>0.20833333333333001</v>
+        <v>0.125</v>
       </c>
       <c r="M37" s="32" t="s">
         <v>15</v>
@@ -8905,11 +8908,11 @@
       </c>
       <c r="AD37" s="1">
         <f>COUNTIF(Difficulte,W18)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AE37" s="19">
         <f>SUMIFS(Duree, Difficulte,W18)</f>
-        <v>2.1666666666666896</v>
+        <v>2.2500000000000231</v>
       </c>
     </row>
     <row r="38" spans="3:31" x14ac:dyDescent="0.2">
@@ -8917,31 +8920,31 @@
         <v>23</v>
       </c>
       <c r="D38" s="40" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E38" s="40"/>
       <c r="F38" s="40"/>
       <c r="G38" s="40"/>
       <c r="H38" s="34">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="I38" s="34" t="s">
         <v>17</v>
       </c>
       <c r="J38" s="34">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K38" s="34">
         <v>2</v>
       </c>
       <c r="L38" s="35">
-        <v>8.3333333333333398E-2</v>
+        <v>0.20833333333333001</v>
       </c>
       <c r="M38" s="34" t="s">
         <v>15</v>
       </c>
       <c r="N38" s="34" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="T38" s="1" t="b">
         <f t="shared" si="1"/>
@@ -8970,7 +8973,7 @@
         <v>24</v>
       </c>
       <c r="D39" s="43" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="E39" s="43"/>
       <c r="F39" s="43"/>
@@ -8988,13 +8991,13 @@
         <v>2</v>
       </c>
       <c r="L39" s="33">
-        <v>6.25E-2</v>
+        <v>8.3333333333333398E-2</v>
       </c>
       <c r="M39" s="32" t="s">
         <v>15</v>
       </c>
       <c r="N39" s="32" t="s">
-        <v>21</v>
+        <v>73</v>
       </c>
       <c r="T39" s="1" t="b">
         <f t="shared" si="1"/>
@@ -9012,13 +9015,13 @@
         <v>25</v>
       </c>
       <c r="D40" s="40" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="E40" s="40"/>
       <c r="F40" s="40"/>
       <c r="G40" s="40"/>
       <c r="H40" s="34">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="I40" s="34" t="s">
         <v>17</v>
@@ -9030,7 +9033,7 @@
         <v>2</v>
       </c>
       <c r="L40" s="35">
-        <v>0.14583333333333401</v>
+        <v>6.25E-2</v>
       </c>
       <c r="M40" s="34" t="s">
         <v>15</v>
@@ -9060,25 +9063,25 @@
         <v>26</v>
       </c>
       <c r="D41" s="43" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="E41" s="43"/>
       <c r="F41" s="43"/>
       <c r="G41" s="43"/>
       <c r="H41" s="32">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="I41" s="32" t="s">
         <v>17</v>
       </c>
       <c r="J41" s="32">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K41" s="32">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L41" s="33">
-        <v>0.33333333333335002</v>
+        <v>0.14583333333333401</v>
       </c>
       <c r="M41" s="32" t="s">
         <v>15</v>
@@ -9101,11 +9104,11 @@
       </c>
       <c r="AD41" s="1">
         <f>COUNTIF(Incertitude,X17)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AE41" s="19">
         <f>SUMIFS(Duree, Incertitude,X17)</f>
-        <v>2.3437500000000249</v>
+        <v>2.4270833333333579</v>
       </c>
     </row>
     <row r="42" spans="3:31" x14ac:dyDescent="0.2">
@@ -9113,25 +9116,25 @@
         <v>27</v>
       </c>
       <c r="D42" s="40" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="E42" s="40"/>
       <c r="F42" s="40"/>
       <c r="G42" s="40"/>
       <c r="H42" s="34">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="I42" s="34" t="s">
         <v>17</v>
       </c>
       <c r="J42" s="34">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K42" s="34">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L42" s="35">
-        <v>0.125</v>
+        <v>0.33333333333335002</v>
       </c>
       <c r="M42" s="34" t="s">
         <v>15</v>
@@ -9166,7 +9169,7 @@
         <v>28</v>
       </c>
       <c r="D43" s="43" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E43" s="43"/>
       <c r="F43" s="43"/>
@@ -9184,13 +9187,13 @@
         <v>1</v>
       </c>
       <c r="L43" s="33">
-        <v>0.13541666666666699</v>
+        <v>0.125</v>
       </c>
       <c r="M43" s="32" t="s">
         <v>15</v>
       </c>
       <c r="N43" s="32" t="s">
-        <v>73</v>
+        <v>21</v>
       </c>
       <c r="T43" s="1" t="b">
         <f t="shared" si="1"/>
@@ -9219,13 +9222,13 @@
         <v>29</v>
       </c>
       <c r="D44" s="40" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E44" s="40"/>
       <c r="F44" s="40"/>
       <c r="G44" s="40"/>
       <c r="H44" s="34">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="I44" s="34" t="s">
         <v>17</v>
@@ -9237,7 +9240,7 @@
         <v>1</v>
       </c>
       <c r="L44" s="35">
-        <v>0.125</v>
+        <v>0.13541666666666699</v>
       </c>
       <c r="M44" s="34" t="s">
         <v>15</v>
@@ -9261,13 +9264,13 @@
         <v>30</v>
       </c>
       <c r="D45" s="43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E45" s="43"/>
       <c r="F45" s="43"/>
       <c r="G45" s="43"/>
       <c r="H45" s="32">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="I45" s="32" t="s">
         <v>17</v>
@@ -9279,13 +9282,13 @@
         <v>1</v>
       </c>
       <c r="L45" s="33">
-        <v>0.14583333333333401</v>
+        <v>0.125</v>
       </c>
       <c r="M45" s="32" t="s">
         <v>15</v>
       </c>
       <c r="N45" s="32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="T45" s="1" t="b">
         <f t="shared" si="1"/>
@@ -9303,31 +9306,31 @@
         <v>31</v>
       </c>
       <c r="D46" s="40" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="E46" s="40"/>
       <c r="F46" s="40"/>
       <c r="G46" s="40"/>
       <c r="H46" s="34">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="I46" s="34" t="s">
         <v>17</v>
       </c>
       <c r="J46" s="34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K46" s="34">
         <v>1</v>
       </c>
       <c r="L46" s="35">
-        <v>8.3333333333333398E-2</v>
+        <v>0.14583333333333401</v>
       </c>
       <c r="M46" s="34" t="s">
         <v>15</v>
       </c>
       <c r="N46" s="34" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="T46" s="1" t="b">
         <f>ISBLANK(D46)</f>
@@ -9345,13 +9348,13 @@
         <v>32</v>
       </c>
       <c r="D47" s="29" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E47" s="29"/>
       <c r="F47" s="29"/>
       <c r="G47" s="29"/>
       <c r="H47" s="32">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I47" s="32" t="s">
         <v>17</v>
@@ -9360,7 +9363,7 @@
         <v>2</v>
       </c>
       <c r="K47" s="32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L47" s="33">
         <v>8.3333333333333398E-2</v>
@@ -9387,31 +9390,31 @@
         <v>33</v>
       </c>
       <c r="D48" s="40" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E48" s="40"/>
       <c r="F48" s="40"/>
       <c r="G48" s="40"/>
       <c r="H48" s="34">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="I48" s="34" t="s">
         <v>17</v>
       </c>
       <c r="J48" s="34">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K48" s="34">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L48" s="35">
-        <v>0.125</v>
+        <v>8.3333333333333398E-2</v>
       </c>
       <c r="M48" s="34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N48" s="34" t="s">
-        <v>73</v>
+        <v>21</v>
       </c>
       <c r="T48" s="1" t="b">
         <f t="shared" ref="T48:T65" si="4">ISBLANK(D48)</f>
@@ -9429,31 +9432,31 @@
         <v>34</v>
       </c>
       <c r="D49" s="43" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="E49" s="43"/>
       <c r="F49" s="43"/>
       <c r="G49" s="43"/>
       <c r="H49" s="32">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="I49" s="32" t="s">
         <v>17</v>
       </c>
       <c r="J49" s="32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K49" s="32">
         <v>1</v>
       </c>
       <c r="L49" s="33">
-        <v>0.104166666666667</v>
+        <v>0.125</v>
       </c>
       <c r="M49" s="32" t="s">
         <v>16</v>
       </c>
       <c r="N49" s="32" t="s">
-        <v>21</v>
+        <v>73</v>
       </c>
       <c r="T49" s="1" t="b">
         <f t="shared" si="4"/>
@@ -9474,13 +9477,13 @@
         <v>35</v>
       </c>
       <c r="D50" s="40" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="E50" s="40"/>
       <c r="F50" s="40"/>
       <c r="G50" s="40"/>
       <c r="H50" s="34">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="I50" s="34" t="s">
         <v>17</v>
@@ -9492,13 +9495,13 @@
         <v>1</v>
       </c>
       <c r="L50" s="35">
-        <v>0.14583333333333401</v>
+        <v>0.104166666666667</v>
       </c>
       <c r="M50" s="34" t="s">
         <v>16</v>
       </c>
       <c r="N50" s="34" t="s">
-        <v>73</v>
+        <v>21</v>
       </c>
       <c r="T50" s="1" t="b">
         <f>ISBLANK(D50)</f>
@@ -9519,31 +9522,31 @@
         <v>36</v>
       </c>
       <c r="D51" s="43" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E51" s="43"/>
       <c r="F51" s="43"/>
       <c r="G51" s="43"/>
       <c r="H51" s="32">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="I51" s="32" t="s">
         <v>17</v>
       </c>
       <c r="J51" s="32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K51" s="32">
         <v>1</v>
       </c>
       <c r="L51" s="33">
-        <v>8.3333333333333398E-2</v>
+        <v>0.14583333333333401</v>
       </c>
       <c r="M51" s="32" t="s">
         <v>16</v>
       </c>
       <c r="N51" s="32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="T51" s="1" t="b">
         <f t="shared" si="4"/>
@@ -9564,31 +9567,31 @@
         <v>37</v>
       </c>
       <c r="D52" s="40" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="E52" s="40"/>
       <c r="F52" s="40"/>
       <c r="G52" s="40"/>
       <c r="H52" s="34">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="I52" s="34" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="J52" s="34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K52" s="34">
         <v>1</v>
       </c>
       <c r="L52" s="35">
-        <v>0.125</v>
+        <v>8.3333333333333398E-2</v>
       </c>
       <c r="M52" s="34" t="s">
         <v>16</v>
       </c>
       <c r="N52" s="34" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="T52" s="1" t="b">
         <f t="shared" si="4"/>
@@ -9609,25 +9612,25 @@
         <v>38</v>
       </c>
       <c r="D53" s="43" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="E53" s="43"/>
       <c r="F53" s="43"/>
       <c r="G53" s="43"/>
       <c r="H53" s="32">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="I53" s="32" t="s">
         <v>12</v>
       </c>
       <c r="J53" s="32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K53" s="32">
         <v>1</v>
       </c>
       <c r="L53" s="33">
-        <v>0.104166666666667</v>
+        <v>0.125</v>
       </c>
       <c r="M53" s="32" t="s">
         <v>16</v>
@@ -9654,25 +9657,25 @@
         <v>39</v>
       </c>
       <c r="D54" s="40" t="s">
-        <v>111</v>
+        <v>87</v>
       </c>
       <c r="E54" s="40"/>
       <c r="F54" s="40"/>
       <c r="G54" s="40"/>
       <c r="H54" s="34">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="I54" s="34" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="J54" s="34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K54" s="34">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L54" s="35">
-        <v>0.125</v>
+        <v>0.104166666666667</v>
       </c>
       <c r="M54" s="34" t="s">
         <v>16</v>
@@ -9698,20 +9701,36 @@
       <c r="C55" s="12">
         <v>40</v>
       </c>
-      <c r="D55" s="43"/>
+      <c r="D55" s="43" t="s">
+        <v>111</v>
+      </c>
       <c r="E55" s="43"/>
       <c r="F55" s="43"/>
       <c r="G55" s="43"/>
-      <c r="H55" s="32"/>
-      <c r="I55" s="32"/>
-      <c r="J55" s="32"/>
-      <c r="K55" s="32"/>
-      <c r="L55" s="33"/>
-      <c r="M55" s="32"/>
-      <c r="N55" s="32"/>
+      <c r="H55" s="32">
+        <v>13</v>
+      </c>
+      <c r="I55" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="J55" s="32">
+        <v>2</v>
+      </c>
+      <c r="K55" s="32">
+        <v>3</v>
+      </c>
+      <c r="L55" s="33">
+        <v>0.125</v>
+      </c>
+      <c r="M55" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="N55" s="32" t="s">
+        <v>21</v>
+      </c>
       <c r="T55" s="1" t="b">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U55" s="2">
         <v>39</v>
@@ -10086,7 +10105,7 @@
     <row r="68" spans="3:25" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="D68" s="1">
         <f>COUNTA(D16:D65)</f>
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H68" s="2"/>
       <c r="I68" s="2"/>
@@ -10094,7 +10113,7 @@
       <c r="K68" s="2"/>
       <c r="L68" s="9">
         <f>SUM(L16:L65)</f>
-        <v>6.302083333329473</v>
+        <v>6.3854166666628061</v>
       </c>
       <c r="M68" s="2"/>
       <c r="N68" s="2"/>
@@ -10589,7 +10608,7 @@
       </c>
       <c r="D5" s="8">
         <f>COUNTIF(Sprint,D4)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E5" s="8">
         <f>COUNTIF(Sprint,E4)</f>
@@ -10601,7 +10620,7 @@
       </c>
       <c r="G5" s="25">
         <f>SUM(C5:F5)</f>
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
@@ -10614,7 +10633,7 @@
       </c>
       <c r="D6" s="10">
         <f>SUMIFS(Duree, Sprint,D4)</f>
-        <v>1.7499999999999978</v>
+        <v>1.8333333333333313</v>
       </c>
       <c r="E6" s="10">
         <f>SUMIFS(Duree, Sprint,E4)</f>
@@ -10626,7 +10645,7 @@
       </c>
       <c r="G6" s="26">
         <f>SUM(C6:F6)</f>
-        <v>6.3020833333294748</v>
+        <v>6.3854166666628078</v>
       </c>
     </row>
     <row r="9" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>